<commit_message>
Version 0.6.2 (or so) - More special levels, more actors, profession selection and backstories, QOL changes like target HP info; also groundwork for conversation (as a single JSON file so far).
</commit_message>
<xml_diff>
--- a/assets/lor_entities.xlsx
+++ b/assets/lor_entities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>Ancient</t>
+  </si>
+  <si>
+    <t>very high AR, low HP</t>
+  </si>
+  <si>
+    <t>^ like RS barrows</t>
   </si>
 </sst>
 </file>
@@ -472,7 +481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,6 +500,8 @@
     <col min="1" max="1" width="41.140625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -801,6 +812,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
+        <v>45</v>
+      </c>
       <c r="P10" s="1" t="s">
         <v>37</v>
       </c>
@@ -828,6 +851,9 @@
       <c r="H11">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>46</v>
       </c>
       <c r="P11" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
XP and leveling, more enemies, facing, special AI and factions, natural weapons, new combat calculator, new quest triggers, item materials and traits, better pack management.
</commit_message>
<xml_diff>
--- a/assets/lor_entities.xlsx
+++ b/assets/lor_entities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -161,13 +161,238 @@
   </si>
   <si>
     <t>^ like RS barrows</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Dark Grey</t>
+  </si>
+  <si>
+    <t>Light Grey</t>
+  </si>
+  <si>
+    <t>Light Blue</t>
+  </si>
+  <si>
+    <t>Light Green</t>
+  </si>
+  <si>
+    <t>Light Cyan</t>
+  </si>
+  <si>
+    <t>Light Red</t>
+  </si>
+  <si>
+    <t>Light Magenta</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>Coaligned</t>
+  </si>
+  <si>
+    <t>Wanderer</t>
+  </si>
+  <si>
+    <t>Elder</t>
+  </si>
+  <si>
+    <t>Physician</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Archaeologist</t>
+  </si>
+  <si>
+    <t>Weaponsmith</t>
+  </si>
+  <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Chaplain</t>
+  </si>
+  <si>
+    <t>Squad Leader</t>
+  </si>
+  <si>
+    <t>Humanoid</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Rogue</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Giant Rat</t>
+  </si>
+  <si>
+    <t>Rat King</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Giant Bat</t>
+  </si>
+  <si>
+    <t>Snakes/Scorpions</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Scorpion</t>
+  </si>
+  <si>
+    <t>Rattlesnake</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Fox</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Wildman</t>
+  </si>
+  <si>
+    <t>Insect</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Giant Beetle</t>
+  </si>
+  <si>
+    <t>Lizard</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Dark Blue</t>
+  </si>
+  <si>
+    <t>Dark Green</t>
+  </si>
+  <si>
+    <t>Dark Cyan</t>
+  </si>
+  <si>
+    <t>Dark Red</t>
+  </si>
+  <si>
+    <t>Dark Magenta</t>
+  </si>
+  <si>
+    <t>Bandit</t>
+  </si>
+  <si>
+    <t>Maniac</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Worm</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Worm Mass</t>
+  </si>
+  <si>
+    <t>Goblin Carver</t>
+  </si>
+  <si>
+    <t>Undead</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Skeleton</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Ogre</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Shadow Knight</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Deserter</t>
+  </si>
+  <si>
+    <t>Cave Crawler</t>
+  </si>
+  <si>
+    <t>Shadow Slave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,13 +408,111 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,17 +527,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF808080"/>
+      <color rgb="FF808000"/>
+      <color rgb="FF800080"/>
+      <color rgb="FF800000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -481,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -491,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -954,20 +1348,309 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="13.7109375" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="20"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="R13" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="R14" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>